<commit_message>
Added Bill of Materials
</commit_message>
<xml_diff>
--- a/Resources/Material List/BOM.xlsx
+++ b/Resources/Material List/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>DHT22</t>
   </si>
@@ -48,6 +48,21 @@
   </si>
   <si>
     <t>Barometer</t>
+  </si>
+  <si>
+    <t>HC-SR501</t>
+  </si>
+  <si>
+    <t>LDR</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>ACS712</t>
+  </si>
+  <si>
+    <t>SRD-05VDC-SL-C</t>
   </si>
 </sst>
 </file>
@@ -402,7 +417,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,6 +437,9 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -432,20 +450,32 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>